<commit_message>
refactoring and naming files and directory
</commit_message>
<xml_diff>
--- a/data/plant_optimization_results.xlsx
+++ b/data/plant_optimization_results.xlsx
@@ -907,86 +907,86 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>29.26060168082566</v>
+        <v>9.792375320235159</v>
       </c>
       <c r="C2">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D2">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>28.64803647229185</v>
+        <v>7.437532810673214</v>
       </c>
       <c r="C3">
+        <v>14</v>
+      </c>
+      <c r="D3">
         <v>30</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>9.792375320235159</v>
+        <v>28.64803647229185</v>
       </c>
       <c r="C4">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="D4">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>8.049427243199435</v>
+        <v>29.26060168082566</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="D5">
-        <v>9</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>8.777835146452022</v>
+        <v>8.049427243199435</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>7.437532810673214</v>
+        <v>8.777835146452022</v>
       </c>
       <c r="C7">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>